<commit_message>
feat: tratamento concluído FEVEREIRO 2023
</commit_message>
<xml_diff>
--- a/Base de Dados/Dados Tratados/JANEIRO_2023.xlsx
+++ b/Base de Dados/Dados Tratados/JANEIRO_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\GitHub\Projeto-Painel-de-BI-Dados-Agricolas\Base de Dados\Dados Tratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F421E610-AAA9-42AC-AEA0-733095BD26DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB056BF-8414-4156-9077-64A0759EAADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AREA_POR_PRODUTO" sheetId="1" r:id="rId1"/>
@@ -13741,9 +13741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A92389E-F363-478C-8FE0-DB1A38F4DB64}">
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ25" sqref="B2:AJ25"/>
+      <selection pane="topRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16757,7 +16757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37856A1E-82E7-45AE-A2B0-C510B7D63887}">
   <dimension ref="A1:AM36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Y36" sqref="B2:Y36"/>
     </sheetView>

</xml_diff>